<commit_message>
update miscellaneous for medi
</commit_message>
<xml_diff>
--- a/meditations/operation/start/start.xlsx
+++ b/meditations/operation/start/start.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t xml:space="preserve">start item </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +71,26 @@
   </si>
   <si>
     <t>金瑞快期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>910097(苏艳辉)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>910101(孙悦)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>052927</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -78,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +113,11 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -123,18 +148,29 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -166,7 +202,7 @@
   </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="start item "/>
-    <tableColumn id="6" name="password"/>
+    <tableColumn id="6" name="password" dataDxfId="0"/>
     <tableColumn id="2" name="group"/>
     <tableColumn id="3" name="shortcut"/>
     <tableColumn id="4" name="exchange"/>
@@ -461,16 +497,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.21875" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -481,7 +517,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
@@ -501,7 +537,7 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
@@ -515,7 +551,7 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>158249</v>
       </c>
       <c r="C3" t="s">
@@ -525,6 +561,43 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="36.6" customHeight="1">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3">
+        <v>300427</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="37.799999999999997" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -536,6 +609,8 @@
   <oleObjects>
     <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1025"/>
     <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1026"/>
+    <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1027"/>
+    <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1028"/>
   </oleObjects>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
update startegy settings and so files for Medi
</commit_message>
<xml_diff>
--- a/meditations/operation/start/start.xlsx
+++ b/meditations/operation/start/start.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,47 +58,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>交易客户端</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shfe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金瑞快期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>052927</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>910096(苏艳利)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>交易客户端</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shfe</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>金瑞快期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>910097(苏艳辉)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>910101(孙悦)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>052927</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,11 +172,185 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1143000</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>361950</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>523875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Object 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Object 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Object 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <oleLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" progId="Package">
     <oleItems>
       <oleItem name="'" icon="1" preferPic="1"/>
@@ -186,10 +360,10 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <oleLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" progId="Package">
     <oleItems>
-      <oleItem name="'" icon="1" preferPic="1"/>
+      <oleItem name="'" advise="1" preferPic="1"/>
     </oleItems>
   </oleLink>
 </externalLink>
@@ -197,9 +371,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:F20" totalsRowShown="0">
-  <autoFilter ref="A1:F20">
-    <filterColumn colId="1"/>
-  </autoFilter>
+  <autoFilter ref="A1:F20"/>
   <tableColumns count="6">
     <tableColumn id="1" name="start item "/>
     <tableColumn id="6" name="password" dataDxfId="0"/>
@@ -213,7 +385,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -287,6 +459,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -321,6 +494,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,24 +670,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34.200000000000003" customHeight="1">
+    <row r="2" spans="1:6" ht="34.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -547,84 +721,181 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="49.2" customHeight="1">
+    <row r="3" spans="1:6" ht="49.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3">
         <v>158249</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" ht="36.6" customHeight="1">
+    <row r="4" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>300427</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="37.9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="37.799999999999997" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <oleObjects>
-    <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1025"/>
-    <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1026"/>
-    <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1027"/>
-    <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1028"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1025">
+          <objectPr defaultSize="0" autoPict="0" dde="1" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1143000</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>361950</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="1025"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1026">
+          <objectPr defaultSize="0" autoPict="0" dde="1" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>523875</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1026"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1027">
+          <objectPr defaultSize="0" autoPict="0" dde="1" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1143000</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>523875</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1027"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1028">
+          <objectPr defaultSize="0" autoPict="0" dde="1" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1143000</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>523875</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1028"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -633,12 +904,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update strategy settings and so files for medi
</commit_message>
<xml_diff>
--- a/meditations/operation/start/start.xlsx
+++ b/meditations/operation/start/start.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t xml:space="preserve">start item </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,6 +91,14 @@
   </si>
   <si>
     <t>910101(孙悦)medi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>910110(王栋)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 0910</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -98,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +126,14 @@
       <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -148,7 +164,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -160,6 +176,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -192,8 +211,8 @@
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1143000</xdr:colOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>361950</xdr:rowOff>
         </xdr:to>
@@ -274,10 +293,10 @@
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>523875</xdr:rowOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -315,10 +334,10 @@
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1143000</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>523875</xdr:rowOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -343,6 +362,42 @@
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1085850" cy="476250"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Object 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -671,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C6" sqref="C6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -772,6 +827,23 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -794,8 +866,8 @@
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1143000</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>361950</xdr:rowOff>
               </to>
@@ -809,7 +881,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1026">
+        <oleObject dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1026">
           <objectPr defaultSize="0" autoPict="0" dde="1" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -829,12 +901,12 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1026"/>
+        <oleObject dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1026"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1027">
+        <oleObject dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1027">
           <objectPr defaultSize="0" autoPict="0" dde="1" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -844,22 +916,22 @@
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1143000</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>523875</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1027"/>
+        <oleObject dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1027"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1028">
+        <oleObject dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1028">
           <objectPr defaultSize="0" autoPict="0" dde="1" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -869,17 +941,42 @@
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1143000</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>523875</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Package" dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1028"/>
+        <oleObject dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1028"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1029">
+          <objectPr defaultSize="0" autoPict="0" dde="1" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject dvAspect="DVASPECT_ICON" link="[2]!''''" oleUpdate="OLEUPDATE_ALWAYS" shapeId="1029"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>